<commit_message>
There was a mistake in data, updated the sharepoint list and recreated the excel sheets.
</commit_message>
<xml_diff>
--- a/deliverables.xlsx
+++ b/deliverables.xlsx
@@ -18,7 +18,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\bfarhoudi\AppData\Local\Microsoft\Windows\Temporary Internet Files\Content.IE5\NMA31CL3\owssvr.iqy" keepAlive="1" name="owssvr" type="5" refreshedVersion="4" minRefreshableVersion="3" saveData="1">
+  <connection id="1" odcFile="C:\Users\bfarhoudi\AppData\Local\Microsoft\Windows\Temporary Internet Files\Content.IE5\63ETHHNT\owssvr.iqy" keepAlive="1" name="owssvr" type="5" refreshedVersion="4" minRefreshableVersion="3" saveData="1">
     <dbPr connection="Provider=Microsoft.Office.List.OLEDB.2.0;Data Source=&quot;&quot;;ApplicationName=Excel;Version=12.0.0.0" command="&lt;LIST&gt;&lt;VIEWGUID&gt;{BC00FD7C-ACD9-4252-8B8E-5F6A3A914ED2}&lt;/VIEWGUID&gt;&lt;LISTNAME&gt;{71557B2C-B9DD-4EA6-B355-882D363C0D13}&lt;/LISTNAME&gt;&lt;LISTWEB&gt;https://share.ahsnet.ca/teams/kmqa/_vti_bin&lt;/LISTWEB&gt;&lt;LISTSUBWEB&gt;&lt;/LISTSUBWEB&gt;&lt;ROOTFOLDER&gt;/teams/kmqa/Lists/Deliverables&lt;/ROOTFOLDER&gt;&lt;/LIST&gt;" commandType="5"/>
   </connection>
 </connections>
@@ -261,7 +261,7 @@
     <t>_Starting Over;#32;#Simulation;#40;#Videography;#41</t>
   </si>
   <si>
-    <t>_Starting Over;#24;#Adobe - Captivate;#44;#Camtasia;#45;#Snagit;#46;#Go Animate;#55</t>
+    <t>_Starting Over;#24;#Adobe - Captivate;#44;#Camtasia;#45;#Snagit;#46;#Go Animate;#55;#Soney Vegas;#47</t>
   </si>
 </sst>
 </file>

</xml_diff>